<commit_message>
Merge cell with drawing example
Drawing should be stretched when placed inside merge cell which is stretched.
</commit_message>
<xml_diff>
--- a/Advanced/DoubleProcessing/result.xlsx
+++ b/Advanced/DoubleProcessing/result.xlsx
@@ -1,55 +1,64 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\TemplaterExamples\Advanced\DoubleProcessing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{369C4B3F-04E7-4E95-BE9C-CF4432D76F23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="1605" windowWidth="19095" windowHeight="9435"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="3" r:id="rId1"/>
     <sheet name="Terran units" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Groups">Report!$A$8:$L$9</definedName>
-    <definedName name="Items">Report!$C$9:$L$9</definedName>
-    <definedName name="temp_range_0">Report!$A$10:$L$13</definedName>
-    <definedName name="temp_range_1">Report!$C$11:$L$11</definedName>
-    <definedName name="temp_range_10">Report!$A$32:$L$36</definedName>
-    <definedName name="temp_range_11">Report!$C$33:$L$33</definedName>
-    <definedName name="temp_range_12">Report!$A$37:$L$40</definedName>
-    <definedName name="temp_range_13">Report!$C$38:$L$38</definedName>
-    <definedName name="temp_range_14">Report!$C$12:$L$12</definedName>
-    <definedName name="temp_range_15">Report!$C$13:$L$13</definedName>
-    <definedName name="temp_range_16">Report!$C$16:$L$16</definedName>
-    <definedName name="temp_range_17">Report!$C$17:$L$17</definedName>
-    <definedName name="temp_range_18">Report!$C$18:$L$18</definedName>
-    <definedName name="temp_range_19">Report!$C$21:$L$21</definedName>
-    <definedName name="temp_range_2">Report!$A$14:$L$18</definedName>
-    <definedName name="temp_range_20">Report!$C$24:$L$24</definedName>
-    <definedName name="temp_range_21">Report!$C$25:$L$25</definedName>
-    <definedName name="temp_range_22">Report!$C$26:$L$26</definedName>
-    <definedName name="temp_range_23">Report!$C$29:$L$29</definedName>
-    <definedName name="temp_range_24">Report!$C$30:$L$30</definedName>
-    <definedName name="temp_range_25">Report!$C$31:$L$31</definedName>
-    <definedName name="temp_range_26">Report!$C$34:$L$34</definedName>
-    <definedName name="temp_range_27">Report!$C$35:$L$35</definedName>
-    <definedName name="temp_range_28">Report!$C$36:$L$36</definedName>
-    <definedName name="temp_range_29">Report!$C$39:$L$39</definedName>
-    <definedName name="temp_range_3">Report!$C$15:$L$15</definedName>
-    <definedName name="temp_range_30">Report!$C$40:$L$40</definedName>
-    <definedName name="temp_range_31">Report!$A$42:$L$42</definedName>
-    <definedName name="temp_range_32">Report!$A$43:$L$43</definedName>
-    <definedName name="temp_range_33">Report!$A$44:$L$44</definedName>
-    <definedName name="temp_range_4">Report!$A$19:$L$21</definedName>
-    <definedName name="temp_range_5">Report!$C$20:$L$20</definedName>
-    <definedName name="temp_range_6">Report!$A$22:$L$26</definedName>
-    <definedName name="temp_range_7">Report!$C$23:$L$23</definedName>
-    <definedName name="temp_range_8">Report!$A$27:$L$31</definedName>
-    <definedName name="temp_range_9">Report!$C$28:$L$28</definedName>
-    <definedName name="Total">Report!$A$41:$L$41</definedName>
+    <definedName name="Groups">Report!$A$8:$M$12</definedName>
+    <definedName name="Items">Report!$C$9:$M$9</definedName>
+    <definedName name="temp_range_0">Report!$A$13:$M$16</definedName>
+    <definedName name="temp_range_1">Report!$C$14:$M$14</definedName>
+    <definedName name="temp_range_10">Report!$A$36:$M$38</definedName>
+    <definedName name="temp_range_11">Report!$C$37:$M$37</definedName>
+    <definedName name="temp_range_12">Report!$A$39:$M$40</definedName>
+    <definedName name="temp_range_13">Report!$C$40:$M$40</definedName>
+    <definedName name="temp_range_14">Report!$A$41:$M$43</definedName>
+    <definedName name="temp_range_15">Report!$C$42:$M$42</definedName>
+    <definedName name="temp_range_16">Report!$C$10:$M$10</definedName>
+    <definedName name="temp_range_17">Report!$C$11:$M$11</definedName>
+    <definedName name="temp_range_18">Report!$C$12:$M$12</definedName>
+    <definedName name="temp_range_19">Report!$C$15:$M$15</definedName>
+    <definedName name="temp_range_2">Report!$A$17:$M$21</definedName>
+    <definedName name="temp_range_20">Report!$C$16:$M$16</definedName>
+    <definedName name="temp_range_21">Report!$C$19:$M$19</definedName>
+    <definedName name="temp_range_22">Report!$C$20:$M$20</definedName>
+    <definedName name="temp_range_23">Report!$C$21:$M$21</definedName>
+    <definedName name="temp_range_24">Report!$C$24:$M$24</definedName>
+    <definedName name="temp_range_25">Report!$C$25:$M$25</definedName>
+    <definedName name="temp_range_26">Report!$C$26:$M$26</definedName>
+    <definedName name="temp_range_27">Report!$C$29:$M$29</definedName>
+    <definedName name="temp_range_28">Report!$C$30:$M$30</definedName>
+    <definedName name="temp_range_29">Report!$C$31:$M$31</definedName>
+    <definedName name="temp_range_3">Report!$C$18:$M$18</definedName>
+    <definedName name="temp_range_30">Report!$C$34:$M$34</definedName>
+    <definedName name="temp_range_31">Report!$C$35:$M$35</definedName>
+    <definedName name="temp_range_32">Report!$C$38:$M$38</definedName>
+    <definedName name="temp_range_33">Report!$C$43:$M$43</definedName>
+    <definedName name="temp_range_34">Report!$A$45:$M$45</definedName>
+    <definedName name="temp_range_35">Report!$A$46:$M$46</definedName>
+    <definedName name="temp_range_36">Report!$A$47:$M$47</definedName>
+    <definedName name="temp_range_4">Report!$A$22:$M$26</definedName>
+    <definedName name="temp_range_5">Report!$C$23:$M$23</definedName>
+    <definedName name="temp_range_6">Report!$A$27:$M$31</definedName>
+    <definedName name="temp_range_7">Report!$C$28:$M$28</definedName>
+    <definedName name="temp_range_8">Report!$A$32:$M$35</definedName>
+    <definedName name="temp_range_9">Report!$C$33:$M$33</definedName>
+    <definedName name="Total">Report!$A$44:$M$44</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -62,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="86">
   <si>
     <t>ASSETS</t>
   </si>
@@ -160,27 +169,39 @@
     <t>number 3</t>
   </si>
   <si>
+    <t>account 4  reg 4</t>
+  </si>
+  <si>
+    <t>name 4</t>
+  </si>
+  <si>
+    <t>number 4</t>
+  </si>
+  <si>
     <t>report header</t>
   </si>
   <si>
-    <t>17.1.2020.</t>
+    <t>24.9.2024.</t>
   </si>
   <si>
     <t>group 0</t>
   </si>
   <si>
-    <t>desc 0</t>
-  </si>
-  <si>
     <t>subitem 0 for 0</t>
   </si>
   <si>
+    <t>subitem 1 for 0</t>
+  </si>
+  <si>
+    <t>subitem 2 for 0</t>
+  </si>
+  <si>
+    <t>subitem 3 for 0</t>
+  </si>
+  <si>
     <t>group 1</t>
   </si>
   <si>
-    <t>desc 1</t>
-  </si>
-  <si>
     <t>subitem 0 for 1</t>
   </si>
   <si>
@@ -193,9 +214,6 @@
     <t>group 2</t>
   </si>
   <si>
-    <t>desc 2</t>
-  </si>
-  <si>
     <t>subitem 0 for 2</t>
   </si>
   <si>
@@ -211,21 +229,21 @@
     <t>group 3</t>
   </si>
   <si>
-    <t>desc 3</t>
-  </si>
-  <si>
     <t>subitem 0 for 3</t>
   </si>
   <si>
     <t>subitem 1 for 3</t>
   </si>
   <si>
+    <t>subitem 2 for 3</t>
+  </si>
+  <si>
+    <t>subitem 3 for 3</t>
+  </si>
+  <si>
     <t>group 4</t>
   </si>
   <si>
-    <t>desc 4</t>
-  </si>
-  <si>
     <t>subitem 0 for 4</t>
   </si>
   <si>
@@ -241,9 +259,6 @@
     <t>group 5</t>
   </si>
   <si>
-    <t>desc 5</t>
-  </si>
-  <si>
     <t>subitem 0 for 5</t>
   </si>
   <si>
@@ -253,40 +268,28 @@
     <t>subitem 2 for 5</t>
   </si>
   <si>
-    <t>subitem 3 for 5</t>
-  </si>
-  <si>
     <t>group 6</t>
   </si>
   <si>
-    <t>desc 6</t>
-  </si>
-  <si>
     <t>subitem 0 for 6</t>
   </si>
   <si>
     <t>subitem 1 for 6</t>
   </si>
   <si>
-    <t>subitem 2 for 6</t>
-  </si>
-  <si>
-    <t>subitem 3 for 6</t>
-  </si>
-  <si>
     <t>group 7</t>
   </si>
   <si>
-    <t>desc 7</t>
-  </si>
-  <si>
     <t>subitem 0 for 7</t>
   </si>
   <si>
-    <t>subitem 1 for 7</t>
-  </si>
-  <si>
-    <t>subitem 2 for 7</t>
+    <t>group 8</t>
+  </si>
+  <si>
+    <t>subitem 0 for 8</t>
+  </si>
+  <si>
+    <t>subitem 1 for 8</t>
   </si>
   <si>
     <t>total 0</t>
@@ -331,7 +334,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="[$-1010409]mmmm\ dd\,\ yyyy"/>
@@ -341,7 +344,7 @@
     <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -981,12 +984,12 @@
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency 2" xfId="5"/>
+    <cellStyle name="Currency 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="6"/>
+    <cellStyle name="Percent 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -1203,19 +1206,591 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38099" y="2124075"/>
+          <a:ext cx="1228725" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hr-HR" sz="1100"/>
+            <a:t>desc 0</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38099" y="2124075"/>
+          <a:ext cx="1228725" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hr-HR" sz="1100"/>
+            <a:t>desc 1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38099" y="2124075"/>
+          <a:ext cx="1228725" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hr-HR" sz="1100"/>
+            <a:t>desc 2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38099" y="2124075"/>
+          <a:ext cx="1228725" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hr-HR" sz="1100"/>
+            <a:t>desc 3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38099" y="2124075"/>
+          <a:ext cx="1228725" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hr-HR" sz="1100"/>
+            <a:t>desc 4</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38099" y="2124075"/>
+          <a:ext cx="1228725" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hr-HR" sz="1100"/>
+            <a:t>desc 5</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38099" y="2124075"/>
+          <a:ext cx="1228725" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hr-HR" sz="1100"/>
+            <a:t>desc 6</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38099" y="2124075"/>
+          <a:ext cx="1228725" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hr-HR" sz="1100"/>
+            <a:t>desc 7</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38099" y="2124075"/>
+          <a:ext cx="1228725" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hr-HR" sz="1100"/>
+            <a:t>desc 8</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I7" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I7" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Unit" dataDxfId="8"/>
-    <tableColumn id="2" name="Size" dataDxfId="7"/>
-    <tableColumn id="3" name="Version" dataDxfId="6"/>
-    <tableColumn id="4" name="Minerals" dataDxfId="5"/>
-    <tableColumn id="5" name="Gas" dataDxfId="4"/>
-    <tableColumn id="6" name="Ground Attack" dataDxfId="3"/>
-    <tableColumn id="7" name="Air Attack" dataDxfId="2"/>
-    <tableColumn id="8" name="Range" dataDxfId="1"/>
-    <tableColumn id="9" name="Build Time" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Unit" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Size" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Version" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Minerals" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Gas" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Ground Attack" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Air Attack" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Range" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Build Time" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1264,7 +1839,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1296,9 +1871,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1330,6 +1923,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1505,21 +2116,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AC75BEC-5E49-4669-9B01-342943DE3302}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView showFormulas="1" showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:C1"/>
-      <selection pane="topRight" sqref="A1:C1"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="5" style="2" customWidth="1"/>
@@ -1533,9 +2143,9 @@
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.5" customHeight="1">
+    <row r="1" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -1546,7 +2156,7 @@
       <c r="H1" s="51"/>
       <c r="I1" s="51"/>
     </row>
-    <row r="2" spans="1:12" ht="13.5" customHeight="1">
+    <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
@@ -1555,9 +2165,9 @@
       <c r="F2" s="4"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="19.5" customHeight="1" thickBot="1">
+    <row r="3" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1568,7 +2178,7 @@
       <c r="H3" s="49"/>
       <c r="I3" s="49"/>
     </row>
-    <row r="4" spans="1:12" ht="2.25" hidden="1" customHeight="1" thickBot="1">
+    <row r="4" spans="1:13" ht="2.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
@@ -1577,7 +2187,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="54.75" customHeight="1">
+    <row r="5" spans="1:13" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="52" t="s">
         <v>0</v>
       </c>
@@ -1595,23 +2205,26 @@
       <c r="G5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="61" t="s">
+      <c r="H5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="61" t="s">
+      <c r="J5" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="61" t="s">
+      <c r="K5" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="61" t="s">
+      <c r="L5" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="61" t="s">
+      <c r="M5" s="61" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1">
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="55"/>
       <c r="B6" s="56"/>
       <c r="C6" s="57"/>
@@ -1627,13 +2240,16 @@
       <c r="G6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="62"/>
+      <c r="H6" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="I6" s="62"/>
       <c r="J6" s="62"/>
       <c r="K6" s="62"/>
       <c r="L6" s="62"/>
-    </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" thickBot="1">
+      <c r="M6" s="62"/>
+    </row>
+    <row r="7" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="58"/>
       <c r="B7" s="59"/>
       <c r="C7" s="60"/>
@@ -1649,1600 +2265,1842 @@
       <c r="G7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="63"/>
+      <c r="H7" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="I7" s="63"/>
       <c r="J7" s="63"/>
       <c r="K7" s="63"/>
       <c r="L7" s="63"/>
-    </row>
-    <row r="8" spans="1:12" ht="21.75" customHeight="1" thickBot="1">
+      <c r="M7" s="63"/>
+    </row>
+    <row r="8" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B8" s="34"/>
       <c r="C8" s="35"/>
       <c r="D8" s="10">
-        <v>5562</v>
+        <v>2083</v>
       </c>
       <c r="E8" s="10">
-        <v>6821</v>
+        <v>4518</v>
       </c>
       <c r="F8" s="10">
-        <v>3813</v>
+        <v>5351</v>
       </c>
       <c r="G8" s="10">
-        <v>1766</v>
-      </c>
-      <c r="H8" s="11">
-        <f t="shared" ref="H8:H45" si="0">SUM(D8:G8)</f>
-        <v>17962</v>
-      </c>
-      <c r="I8" s="12">
-        <f t="shared" ref="I8:I40" si="1">H8/H$45</f>
-        <v>0.12281289528563126</v>
-      </c>
-      <c r="J8" s="13">
-        <v>2.0052712140629398</v>
+        <v>4672</v>
+      </c>
+      <c r="H8" s="10">
+        <v>7532</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" ref="I8:I48" si="0">SUM(D8:H8)</f>
+        <v>24156</v>
+      </c>
+      <c r="J8" s="12">
+        <f t="shared" ref="J8:J43" si="1">I8/I$48</f>
+        <v>0.10938037709876655</v>
       </c>
       <c r="K8" s="13">
-        <f>IF( 1.70577596952476&gt;0,2.00527121406294 + (2.00527121406294 * 1.70577596952476),0)</f>
-        <v>5.4258146633912432</v>
-      </c>
-      <c r="L8" s="14">
-        <f t="shared" ref="L8:L40" si="2">(J8*H$45)-H8</f>
-        <v>275318.94141277525</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A9" s="47" t="s">
-        <v>35</v>
-      </c>
+        <v>0.61474832269118596</v>
+      </c>
+      <c r="L8" s="13">
+        <f>IF( 80.3170954251276&gt;0,0.614748322691186 + (0.614748322691186 * 80.3170954251276),0)</f>
+        <v>49.989548018716306</v>
+      </c>
+      <c r="M8" s="14">
+        <f t="shared" ref="M8:M43" si="2">(K8*I$48)-I8</f>
+        <v>111607.47857641228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="47"/>
       <c r="B9" s="48"/>
       <c r="C9" s="15" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D9" s="16">
-        <v>1889</v>
+        <v>3692</v>
       </c>
       <c r="E9" s="16">
-        <v>3070</v>
+        <v>4759</v>
       </c>
       <c r="F9" s="16">
-        <v>1324</v>
+        <v>9529</v>
       </c>
       <c r="G9" s="16">
-        <v>3850</v>
+        <v>179</v>
       </c>
       <c r="H9" s="16">
+        <v>4034</v>
+      </c>
+      <c r="I9" s="16">
         <f t="shared" si="0"/>
-        <v>10133</v>
-      </c>
-      <c r="I9" s="17">
+        <v>22193</v>
+      </c>
+      <c r="J9" s="17">
         <f t="shared" si="1"/>
-        <v>6.9283101432429661E-2</v>
-      </c>
-      <c r="J9" s="18">
-        <v>0.15089949506842501</v>
+        <v>0.10049174983246092</v>
       </c>
       <c r="K9" s="18">
-        <f>IF( 5.41167204054616&gt;0,0.150899495068425 +(0.150899495068425*67.1532092463007),0)</f>
-        <v>10.28428486255949</v>
-      </c>
-      <c r="L9" s="19">
+        <v>0.53537103232712102</v>
+      </c>
+      <c r="L9" s="18">
+        <f>IF( 5.45892966699737&gt;0,0.535371032327121 +(0.535371032327121*18.8859419519482),0)</f>
+        <v>10.646357271611713</v>
+      </c>
+      <c r="M9" s="19">
         <f t="shared" si="2"/>
-        <v>11936.805651232498</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A10" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="10">
-        <v>8760</v>
-      </c>
-      <c r="E10" s="10">
-        <v>3174</v>
-      </c>
-      <c r="F10" s="10">
-        <v>854</v>
-      </c>
-      <c r="G10" s="10">
-        <v>1676</v>
-      </c>
-      <c r="H10" s="11">
+        <v>96040.48026325072</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="16">
+        <v>5739</v>
+      </c>
+      <c r="E10" s="16">
+        <v>3373</v>
+      </c>
+      <c r="F10" s="16">
+        <v>3400</v>
+      </c>
+      <c r="G10" s="16">
+        <v>1287</v>
+      </c>
+      <c r="H10" s="16">
+        <v>7645</v>
+      </c>
+      <c r="I10" s="16">
         <f t="shared" si="0"/>
-        <v>14464</v>
-      </c>
-      <c r="I10" s="12">
+        <v>21444</v>
+      </c>
+      <c r="J10" s="17">
         <f t="shared" si="1"/>
-        <v>9.8895764247376158E-2</v>
-      </c>
-      <c r="J10" s="13">
-        <v>5.5192029362168196</v>
-      </c>
-      <c r="K10" s="13">
-        <f>IF( 74.0886007780622&gt;0,5.51920293621682 + (5.51920293621682 * 74.0886007780622),0)</f>
-        <v>414.42922589069343</v>
-      </c>
-      <c r="L10" s="14">
+        <v>9.7100215536758974E-2</v>
+      </c>
+      <c r="K10" s="18">
+        <v>7.1447981089096502E-2</v>
+      </c>
+      <c r="L10" s="18">
+        <f>IF( 6.346515447994&gt;0,0.0714479810890965 +(0.0714479810890965*74.7610078075719),0)</f>
+        <v>5.4129710531262889</v>
+      </c>
+      <c r="M10" s="19">
         <f t="shared" si="2"/>
-        <v>792747.02543639089</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A11" s="47" t="s">
-        <v>38</v>
-      </c>
+        <v>-5665.142064359572</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="47"/>
       <c r="B11" s="48"/>
       <c r="C11" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D11" s="16">
-        <v>5087</v>
+        <v>3290</v>
       </c>
       <c r="E11" s="16">
-        <v>6085</v>
+        <v>1615</v>
       </c>
       <c r="F11" s="16">
-        <v>4587</v>
+        <v>8472</v>
       </c>
       <c r="G11" s="16">
-        <v>3726</v>
+        <v>1644</v>
       </c>
       <c r="H11" s="16">
+        <v>160</v>
+      </c>
+      <c r="I11" s="16">
         <f t="shared" si="0"/>
-        <v>19485</v>
-      </c>
-      <c r="I11" s="17">
+        <v>15181</v>
+      </c>
+      <c r="J11" s="17">
         <f t="shared" si="1"/>
-        <v>0.13322621448839356</v>
-      </c>
-      <c r="J11" s="18">
-        <v>0.12947192701020799</v>
+        <v>6.8740830631577043E-2</v>
       </c>
       <c r="K11" s="18">
-        <f>IF( 8.76748995332396&gt;0,0.129471927010208 +(0.129471927010208*49.909417121629),0)</f>
-        <v>6.591340337703782</v>
-      </c>
-      <c r="L11" s="19">
+        <v>0.71969021610901196</v>
+      </c>
+      <c r="L11" s="18">
+        <f>IF( 4.97826152712957&gt;0,0.719690216109012 +(0.719690216109012*38.5129646577467),0)</f>
+        <v>28.437094073641475</v>
+      </c>
+      <c r="M11" s="19">
         <f t="shared" si="2"/>
-        <v>-549.08331512203222</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="22.5" customHeight="1">
+        <v>143758.26608637863</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="48"/>
       <c r="C12" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="16">
-        <v>7154</v>
+        <v>1941</v>
       </c>
       <c r="E12" s="16">
-        <v>5196</v>
+        <v>8586</v>
       </c>
       <c r="F12" s="16">
-        <v>2943</v>
+        <v>2258</v>
       </c>
       <c r="G12" s="16">
-        <v>4009</v>
+        <v>4906</v>
       </c>
       <c r="H12" s="16">
+        <v>6356</v>
+      </c>
+      <c r="I12" s="16">
         <f t="shared" si="0"/>
-        <v>19302</v>
-      </c>
-      <c r="I12" s="17">
+        <v>24047</v>
+      </c>
+      <c r="J12" s="17">
         <f t="shared" si="1"/>
-        <v>0.13197497521452259</v>
-      </c>
-      <c r="J12" s="18">
-        <v>0.13397528190816499</v>
+        <v>0.10888681603303689</v>
       </c>
       <c r="K12" s="18">
-        <f>IF( 7.18794598578845&gt;0,0.133975281908165 +(0.133975281908165*33.0586727396858),0)</f>
-        <v>4.5630202817173382</v>
-      </c>
-      <c r="L12" s="19">
+        <v>0.20960040120855</v>
+      </c>
+      <c r="L12" s="18">
+        <f>IF( 3.52017538320281&gt;0,0.20960040120855 +(0.20960040120855*15.62459278648),0)</f>
+        <v>3.4845213179749739</v>
+      </c>
+      <c r="M12" s="19">
         <f t="shared" si="2"/>
-        <v>292.5548554786692</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A13" s="47"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="16">
-        <v>2241</v>
-      </c>
-      <c r="E13" s="16">
-        <v>8650</v>
-      </c>
-      <c r="F13" s="16">
-        <v>8581</v>
-      </c>
-      <c r="G13" s="16">
-        <v>2744</v>
-      </c>
-      <c r="H13" s="16">
+        <v>22241.991004501018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="10">
+        <v>7863</v>
+      </c>
+      <c r="E13" s="10">
+        <v>8248</v>
+      </c>
+      <c r="F13" s="10">
+        <v>7627</v>
+      </c>
+      <c r="G13" s="10">
+        <v>852</v>
+      </c>
+      <c r="H13" s="10">
+        <v>8922</v>
+      </c>
+      <c r="I13" s="11">
         <f t="shared" si="0"/>
-        <v>22216</v>
-      </c>
-      <c r="I13" s="17">
+        <v>33512</v>
+      </c>
+      <c r="J13" s="12">
         <f t="shared" si="1"/>
-        <v>0.15189908037332056</v>
-      </c>
-      <c r="J13" s="18">
-        <v>0.3510750137973</v>
-      </c>
-      <c r="K13" s="18">
-        <f>IF( 4.68771490486698&gt;0,0.3510750137973 +(0.3510750137973*41.8488223766204),0)</f>
-        <v>15.043150907070064</v>
-      </c>
-      <c r="L13" s="19">
+        <v>0.15174512325442394</v>
+      </c>
+      <c r="K13" s="13">
+        <v>6.9710225644386501</v>
+      </c>
+      <c r="L13" s="13">
+        <f>IF( 95.4989995320789&gt;0,6.97102256443865 + (6.97102256443865 * 95.4989995320789),0)</f>
+        <v>672.69670318387671</v>
+      </c>
+      <c r="M13" s="14">
         <f t="shared" si="2"/>
-        <v>29130.476142924112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A14" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="10">
-        <v>5198</v>
-      </c>
-      <c r="E14" s="10">
-        <v>8498</v>
-      </c>
-      <c r="F14" s="10">
-        <v>8144</v>
-      </c>
-      <c r="G14" s="10">
-        <v>588</v>
-      </c>
-      <c r="H14" s="11">
+        <v>1505996.5072208892</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="16">
+        <v>306</v>
+      </c>
+      <c r="E14" s="16">
+        <v>5578</v>
+      </c>
+      <c r="F14" s="16">
+        <v>726</v>
+      </c>
+      <c r="G14" s="16">
+        <v>4295</v>
+      </c>
+      <c r="H14" s="16">
+        <v>6802</v>
+      </c>
+      <c r="I14" s="16">
         <f t="shared" si="0"/>
-        <v>22428</v>
-      </c>
-      <c r="I14" s="12">
+        <v>17707</v>
+      </c>
+      <c r="J14" s="17">
         <f t="shared" si="1"/>
-        <v>0.15334860346654816</v>
-      </c>
-      <c r="J14" s="13">
-        <v>3.1145044477258401</v>
-      </c>
-      <c r="K14" s="13">
-        <f>IF( 69.757305723502&gt;0,3.11450444772584 + (3.11450444772584 * 69.757305723502),0)</f>
-        <v>220.37394338494403</v>
-      </c>
-      <c r="L14" s="14">
+        <v>8.0178768723623922E-2</v>
+      </c>
+      <c r="K14" s="18">
+        <v>0.29719377695452098</v>
+      </c>
+      <c r="L14" s="18">
+        <f>IF( 7.31722973162179&gt;0,0.297193776954521 +(0.297193776954521*5.19334702063042),0)</f>
+        <v>1.8406241930511842</v>
+      </c>
+      <c r="M14" s="19">
         <f t="shared" si="2"/>
-        <v>433083.84800214274</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A15" s="47" t="s">
-        <v>43</v>
-      </c>
+        <v>47926.462477744237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="47"/>
       <c r="B15" s="48"/>
       <c r="C15" s="15" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="16">
-        <v>2991</v>
+        <v>4533</v>
       </c>
       <c r="E15" s="16">
-        <v>400</v>
+        <v>1188</v>
       </c>
       <c r="F15" s="16">
-        <v>6364</v>
+        <v>3703</v>
       </c>
       <c r="G15" s="16">
-        <v>422</v>
+        <v>6151</v>
       </c>
       <c r="H15" s="16">
+        <v>5875</v>
+      </c>
+      <c r="I15" s="16">
         <f t="shared" si="0"/>
-        <v>10177</v>
-      </c>
-      <c r="I15" s="17">
+        <v>21450</v>
+      </c>
+      <c r="J15" s="17">
         <f t="shared" si="1"/>
-        <v>6.9583945848005202E-2</v>
-      </c>
-      <c r="J15" s="18">
-        <v>0.47941046044203001</v>
+        <v>9.7127384035789965E-2</v>
       </c>
       <c r="K15" s="18">
-        <f>IF( 9.79172630691516&gt;0,0.47941046044203 +(0.47941046044203*94.3640126354825),0)</f>
-        <v>45.718505207176236</v>
-      </c>
-      <c r="L15" s="19">
+        <v>0.91972614588203205</v>
+      </c>
+      <c r="L15" s="18">
+        <f>IF( 6.48962515708507&gt;0,0.919726145882032 +(0.919726145882032*97.7576035530109),0)</f>
+        <v>90.829950092356398</v>
+      </c>
+      <c r="M15" s="19">
         <f t="shared" si="2"/>
-        <v>59939.176891949101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="22.5" customHeight="1">
+        <v>181666.00096117149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="48"/>
       <c r="C16" s="15" t="s">
         <v>45</v>
       </c>
       <c r="D16" s="16">
-        <v>2214</v>
+        <v>5682</v>
       </c>
       <c r="E16" s="16">
-        <v>40</v>
+        <v>8238</v>
       </c>
       <c r="F16" s="16">
-        <v>398</v>
+        <v>5447</v>
       </c>
       <c r="G16" s="16">
-        <v>2264</v>
+        <v>3109</v>
       </c>
       <c r="H16" s="16">
+        <v>566</v>
+      </c>
+      <c r="I16" s="16">
         <f t="shared" si="0"/>
-        <v>4916</v>
-      </c>
-      <c r="I16" s="17">
+        <v>23042</v>
+      </c>
+      <c r="J16" s="17">
         <f t="shared" si="1"/>
-        <v>3.3612526067484876E-2</v>
-      </c>
-      <c r="J16" s="18">
-        <v>0.68901662933128704</v>
+        <v>0.10433609244534603</v>
       </c>
       <c r="K16" s="18">
-        <f>IF( 5.91151648476325&gt;0,0.689016629331287 +(0.689016629331287*61.2498162133851),0)</f>
-        <v>42.891158543838706</v>
-      </c>
-      <c r="L16" s="19">
+        <v>0.55355342270506203</v>
+      </c>
+      <c r="L16" s="18">
+        <f>IF( 3.63931809721483&gt;0,0.553553422705062 +(0.553553422705062*98.4672905870095),0)</f>
+        <v>55.060459151638113</v>
+      </c>
+      <c r="M16" s="19">
         <f t="shared" si="2"/>
-        <v>95856.127122847392</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A17" s="47"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="15" t="s">
+        <v>99206.95208387672</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="16">
-        <v>916</v>
-      </c>
-      <c r="E17" s="16">
-        <v>7507</v>
-      </c>
-      <c r="F17" s="16">
-        <v>4077</v>
-      </c>
-      <c r="G17" s="16">
-        <v>9527</v>
-      </c>
-      <c r="H17" s="16">
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="10">
+        <v>8833</v>
+      </c>
+      <c r="E17" s="10">
+        <v>8519</v>
+      </c>
+      <c r="F17" s="10">
+        <v>9253</v>
+      </c>
+      <c r="G17" s="10">
+        <v>5722</v>
+      </c>
+      <c r="H17" s="10">
+        <v>938</v>
+      </c>
+      <c r="I17" s="11">
         <f t="shared" si="0"/>
-        <v>22027</v>
-      </c>
-      <c r="I17" s="17">
+        <v>33265</v>
+      </c>
+      <c r="J17" s="12">
         <f t="shared" si="1"/>
-        <v>0.15060681686096203</v>
-      </c>
-      <c r="J17" s="18">
-        <v>0.221333566224824</v>
-      </c>
-      <c r="K17" s="18">
-        <f>IF( 5.17529605663162&gt;0,0.221333566224824 +(0.221333566224824*66.5498021368635),0)</f>
-        <v>14.951038604733236</v>
-      </c>
-      <c r="L17" s="19">
+        <v>0.15062668671098151</v>
+      </c>
+      <c r="K17" s="13">
+        <v>1.83188260152558</v>
+      </c>
+      <c r="L17" s="13">
+        <f>IF( 43.0737582701602&gt;0,1.83188260152558 + (1.83188260152558 * 43.0737582701602),0)</f>
+        <v>80.737950958950606</v>
+      </c>
+      <c r="M17" s="14">
         <f t="shared" si="2"/>
-        <v>10344.140728211634</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="22.5" customHeight="1">
+        <v>371295.2812513152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="48"/>
       <c r="C18" s="15" t="s">
         <v>47</v>
       </c>
       <c r="D18" s="16">
-        <v>178</v>
+        <v>5774</v>
       </c>
       <c r="E18" s="16">
-        <v>378</v>
+        <v>9853</v>
       </c>
       <c r="F18" s="16">
-        <v>7253</v>
+        <v>1630</v>
       </c>
       <c r="G18" s="16">
-        <v>6907</v>
+        <v>4267</v>
       </c>
       <c r="H18" s="16">
+        <v>9562</v>
+      </c>
+      <c r="I18" s="16">
         <f t="shared" si="0"/>
-        <v>14716</v>
-      </c>
-      <c r="I18" s="17">
+        <v>31086</v>
+      </c>
+      <c r="J18" s="17">
         <f t="shared" si="1"/>
-        <v>0.10061878226385423</v>
-      </c>
-      <c r="J18" s="18">
-        <v>0.119159075487013</v>
+        <v>0.14075999347956022</v>
       </c>
       <c r="K18" s="18">
-        <f>IF( 1.96777282840003&gt;0,0.119159075487013 +(0.119159075487013*91.0552325151187),0)</f>
-        <v>10.969216400243564</v>
-      </c>
-      <c r="L18" s="19">
+        <v>0.51337644342024602</v>
+      </c>
+      <c r="L18" s="18">
+        <f>IF( 5.61342331376552&gt;0,0.513376443420246 +(0.513376443420246*49.3346038504199),0)</f>
+        <v>25.840599905695591</v>
+      </c>
+      <c r="M18" s="19">
         <f t="shared" si="2"/>
-        <v>2711.6105853530862</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A19" s="33" t="s">
+        <v>82290.107270700813</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="10">
-        <v>735</v>
-      </c>
-      <c r="E19" s="10">
-        <v>4552</v>
-      </c>
-      <c r="F19" s="10">
-        <v>9514</v>
-      </c>
-      <c r="G19" s="10">
-        <v>2284</v>
-      </c>
-      <c r="H19" s="11">
+      <c r="D19" s="16">
+        <v>4388</v>
+      </c>
+      <c r="E19" s="16">
+        <v>1833</v>
+      </c>
+      <c r="F19" s="16">
+        <v>925</v>
+      </c>
+      <c r="G19" s="16">
+        <v>9823</v>
+      </c>
+      <c r="H19" s="16">
+        <v>5419</v>
+      </c>
+      <c r="I19" s="16">
         <f t="shared" si="0"/>
-        <v>17085</v>
-      </c>
-      <c r="I19" s="12">
+        <v>22388</v>
+      </c>
+      <c r="J19" s="17">
         <f t="shared" si="1"/>
-        <v>0.11681651909336432</v>
-      </c>
-      <c r="J19" s="13">
-        <v>2.5354955264066801</v>
-      </c>
-      <c r="K19" s="13">
-        <f>IF( 85.7046164505671&gt;0,2.53549552640668 + (2.53549552640668 * 85.7046164505671),0)</f>
-        <v>219.83916712921993</v>
-      </c>
-      <c r="L19" s="14">
+        <v>0.1013747260509681</v>
+      </c>
+      <c r="K19" s="18">
+        <v>0.10992088965602299</v>
+      </c>
+      <c r="L19" s="18">
+        <f>IF( 0.352638494387566&gt;0,0.109920889656023 +(0.109920889656023*54.0291119618477),0)</f>
+        <v>6.0488489438271964</v>
+      </c>
+      <c r="M19" s="19">
         <f t="shared" si="2"/>
-        <v>353743.89821460901</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A20" s="47" t="s">
-        <v>49</v>
-      </c>
+        <v>1887.3689551947427</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="47"/>
       <c r="B20" s="48"/>
       <c r="C20" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="16">
-        <v>7644</v>
+        <v>8068</v>
       </c>
       <c r="E20" s="16">
-        <v>935</v>
+        <v>2559</v>
       </c>
       <c r="F20" s="16">
-        <v>2401</v>
+        <v>9368</v>
       </c>
       <c r="G20" s="16">
-        <v>3520</v>
+        <v>5321</v>
       </c>
       <c r="H20" s="16">
+        <v>5812</v>
+      </c>
+      <c r="I20" s="16">
         <f t="shared" si="0"/>
-        <v>14500</v>
-      </c>
-      <c r="I20" s="17">
+        <v>31128</v>
+      </c>
+      <c r="J20" s="17">
         <f t="shared" si="1"/>
-        <v>9.9141909678301596E-2</v>
-      </c>
-      <c r="J20" s="18">
-        <v>0.27971627576263403</v>
+        <v>0.14095017297277718</v>
       </c>
       <c r="K20" s="18">
-        <f>IF( 6.44176412208088&gt;0,0.279716275762634 +(0.279716275762634*85.4953017483909),0)</f>
-        <v>24.194143676025149</v>
-      </c>
-      <c r="L20" s="19">
+        <v>0.53083578102795204</v>
+      </c>
+      <c r="L20" s="18">
+        <f>IF( 4.76147141063654&gt;0,0.530835781027952 +(0.530835781027952*19.3518702962212),0)</f>
+        <v>10.803500964074157</v>
+      </c>
+      <c r="M20" s="19">
         <f t="shared" si="2"/>
-        <v>26409.903911664042</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="22.5" customHeight="1">
+        <v>86103.897225337045</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="B21" s="48"/>
       <c r="C21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="16">
+        <v>879</v>
+      </c>
+      <c r="E21" s="16">
+        <v>2465</v>
+      </c>
+      <c r="F21" s="16">
+        <v>2499</v>
+      </c>
+      <c r="G21" s="16">
+        <v>4884</v>
+      </c>
+      <c r="H21" s="16">
+        <v>8496</v>
+      </c>
+      <c r="I21" s="16">
+        <f t="shared" si="0"/>
+        <v>19223</v>
+      </c>
+      <c r="J21" s="17">
+        <f t="shared" si="1"/>
+        <v>8.7043342812120769E-2</v>
+      </c>
+      <c r="K21" s="18">
+        <v>0.20147291300886899</v>
+      </c>
+      <c r="L21" s="18">
+        <f>IF( 5.28200163751934&gt;0,0.201472913008869 +(0.201472913008869*54.9956205091419),0)</f>
+        <v>11.281600779715987</v>
+      </c>
+      <c r="M21" s="19">
+        <f t="shared" si="2"/>
+        <v>25271.084000530667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
         <v>51</v>
-      </c>
-      <c r="D21" s="16">
-        <v>2356</v>
-      </c>
-      <c r="E21" s="16">
-        <v>1262</v>
-      </c>
-      <c r="F21" s="16">
-        <v>7799</v>
-      </c>
-      <c r="G21" s="16">
-        <v>8275</v>
-      </c>
-      <c r="H21" s="16">
-        <f t="shared" si="0"/>
-        <v>19692</v>
-      </c>
-      <c r="I21" s="17">
-        <f t="shared" si="1"/>
-        <v>0.13464155071621484</v>
-      </c>
-      <c r="J21" s="18">
-        <v>0.69895228263873199</v>
-      </c>
-      <c r="K21" s="18">
-        <f>IF( 6.06870307869683&gt;0,0.698952282638732 +(0.698952282638732*45.4123860436549),0)</f>
-        <v>32.440043167922617</v>
-      </c>
-      <c r="L21" s="19">
-        <f t="shared" si="2"/>
-        <v>82533.266097327753</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A22" s="33" t="s">
-        <v>52</v>
       </c>
       <c r="B22" s="34"/>
       <c r="C22" s="35"/>
       <c r="D22" s="10">
-        <v>5364</v>
+        <v>9350</v>
       </c>
       <c r="E22" s="10">
-        <v>1077</v>
+        <v>4918</v>
       </c>
       <c r="F22" s="10">
-        <v>2888</v>
+        <v>5559</v>
       </c>
       <c r="G22" s="10">
-        <v>122</v>
-      </c>
-      <c r="H22" s="11">
+        <v>6154</v>
+      </c>
+      <c r="H22" s="10">
+        <v>3171</v>
+      </c>
+      <c r="I22" s="11">
         <f t="shared" si="0"/>
-        <v>9451</v>
-      </c>
-      <c r="I22" s="12">
+        <v>29152</v>
+      </c>
+      <c r="J22" s="12">
         <f t="shared" si="1"/>
-        <v>6.4620012991008849E-2</v>
-      </c>
-      <c r="J22" s="13">
-        <v>1.07791076930142</v>
+        <v>0.13200268062523773</v>
       </c>
       <c r="K22" s="13">
-        <f>IF( 89.5641578312796&gt;0,1.07791076930142 + (1.07791076930142 * 89.5641578312796),0)</f>
-        <v>97.620081039049822</v>
-      </c>
-      <c r="L22" s="14">
+        <v>2.85055854490518</v>
+      </c>
+      <c r="L22" s="13">
+        <f>IF( 65.8849396118358&gt;0,2.85055854490518 + (2.85055854490518 * 65.8849396118358),0)</f>
+        <v>190.65943613598549</v>
+      </c>
+      <c r="M22" s="14">
         <f t="shared" si="2"/>
-        <v>148198.83956417919</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A23" s="47" t="s">
-        <v>53</v>
-      </c>
+        <v>600376.75129103963</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="47"/>
       <c r="B23" s="48"/>
       <c r="C23" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D23" s="16">
-        <v>3515</v>
+        <v>8171</v>
       </c>
       <c r="E23" s="16">
-        <v>3608</v>
+        <v>6178</v>
       </c>
       <c r="F23" s="16">
-        <v>7826</v>
+        <v>3716</v>
       </c>
       <c r="G23" s="16">
-        <v>340</v>
+        <v>2729</v>
       </c>
       <c r="H23" s="16">
+        <v>33</v>
+      </c>
+      <c r="I23" s="16">
         <f t="shared" si="0"/>
-        <v>15289</v>
-      </c>
-      <c r="I23" s="17">
+        <v>20827</v>
+      </c>
+      <c r="J23" s="17">
         <f t="shared" si="1"/>
-        <v>0.10453659703941745</v>
-      </c>
-      <c r="J23" s="18">
-        <v>0.96715322135349402</v>
+        <v>9.4306388219738815E-2</v>
       </c>
       <c r="K23" s="18">
-        <f>IF( 1.45989727762523&gt;0,0.967153221353494 +(0.967153221353494*75.7765927239212),0)</f>
-        <v>74.254728977485627</v>
-      </c>
-      <c r="L23" s="19">
+        <v>0.64173280151641598</v>
+      </c>
+      <c r="L23" s="18">
+        <f>IF( 3.20816693045579&gt;0,0.641732801516416 +(0.641732801516416*77.4027210555052),0)</f>
+        <v>50.313597829459447</v>
+      </c>
+      <c r="M23" s="19">
         <f t="shared" si="2"/>
-        <v>126161.99438905527</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="22.5" customHeight="1">
+        <v>120895.83881809138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="47"/>
       <c r="B24" s="48"/>
       <c r="C24" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D24" s="16">
-        <v>1623</v>
+        <v>3425</v>
       </c>
       <c r="E24" s="16">
-        <v>2400</v>
+        <v>448</v>
       </c>
       <c r="F24" s="16">
-        <v>6405</v>
+        <v>6696</v>
       </c>
       <c r="G24" s="16">
-        <v>3924</v>
+        <v>6315</v>
       </c>
       <c r="H24" s="16">
+        <v>5534</v>
+      </c>
+      <c r="I24" s="16">
         <f t="shared" si="0"/>
-        <v>14352</v>
-      </c>
-      <c r="I24" s="17">
+        <v>22418</v>
+      </c>
+      <c r="J24" s="17">
         <f t="shared" si="1"/>
-        <v>9.8129978462274794E-2</v>
-      </c>
-      <c r="J24" s="18">
-        <v>0.83614506099193597</v>
+        <v>0.10151056854612306</v>
       </c>
       <c r="K24" s="18">
-        <f>IF( 9.86302588594287&gt;0,0.836145060991936 +(0.836145060991936*31.4522246976626),0)</f>
-        <v>27.134767399151105</v>
-      </c>
-      <c r="L24" s="19">
+        <v>0.37508358730705599</v>
+      </c>
+      <c r="L24" s="18">
+        <f>IF( 0.462354179687032&gt;0,0.375083587307056 +(0.375083587307056*50.9192001311664),0)</f>
+        <v>19.474039835310865</v>
+      </c>
+      <c r="M24" s="19">
         <f t="shared" si="2"/>
-        <v>107938.39589537559</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="22.5" customHeight="1">
+        <v>60416.95975523947</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
       <c r="B25" s="48"/>
       <c r="C25" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D25" s="16">
-        <v>7136</v>
+        <v>9687</v>
       </c>
       <c r="E25" s="16">
-        <v>8700</v>
+        <v>3397</v>
       </c>
       <c r="F25" s="16">
-        <v>2385</v>
+        <v>7107</v>
       </c>
       <c r="G25" s="16">
-        <v>223</v>
+        <v>2648</v>
       </c>
       <c r="H25" s="16">
+        <v>743</v>
+      </c>
+      <c r="I25" s="16">
         <f t="shared" si="0"/>
-        <v>18444</v>
-      </c>
-      <c r="I25" s="17">
+        <v>23582</v>
+      </c>
+      <c r="J25" s="17">
         <f t="shared" si="1"/>
-        <v>0.12610850911079963</v>
-      </c>
-      <c r="J25" s="18">
-        <v>0.16188002105889801</v>
+        <v>0.10678125735813515</v>
       </c>
       <c r="K25" s="18">
-        <f>IF( 8.01981752646147&gt;0,0.161880021058898 +(0.161880021058898*59.9745919741572),0)</f>
-        <v>9.8705682328342821</v>
-      </c>
-      <c r="L25" s="19">
+        <v>0.64381741110413204</v>
+      </c>
+      <c r="L25" s="18">
+        <f>IF( 2.36781055217973&gt;0,0.643817411104132 +(0.643817411104132*65.4332444842128),0)</f>
+        <v>42.770879475073748</v>
+      </c>
+      <c r="M25" s="19">
         <f t="shared" si="2"/>
-        <v>5231.7624799691293</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="22.5" customHeight="1">
+        <v>118601.21233788095</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="47"/>
       <c r="B26" s="48"/>
       <c r="C26" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D26" s="16">
-        <v>9107</v>
+        <v>5421</v>
       </c>
       <c r="E26" s="16">
-        <v>2925</v>
+        <v>6975</v>
       </c>
       <c r="F26" s="16">
-        <v>4983</v>
+        <v>8827</v>
       </c>
       <c r="G26" s="16">
-        <v>3043</v>
+        <v>1007</v>
       </c>
       <c r="H26" s="16">
+        <v>1017</v>
+      </c>
+      <c r="I26" s="16">
         <f t="shared" si="0"/>
-        <v>20058</v>
-      </c>
-      <c r="I26" s="17">
+        <v>23247</v>
+      </c>
+      <c r="J26" s="17">
         <f t="shared" si="1"/>
-        <v>0.1371440292639568</v>
-      </c>
-      <c r="J26" s="18">
-        <v>0.79942569220411897</v>
+        <v>0.10526434949557154</v>
       </c>
       <c r="K26" s="18">
-        <f>IF( 7.49255087575528&gt;0,0.799425692204119 +(0.799425692204119*38.5451276500454),0)</f>
-        <v>31.613391044937789</v>
-      </c>
-      <c r="L26" s="19">
+        <v>5.3568307335287502E-2</v>
+      </c>
+      <c r="L26" s="18">
+        <f>IF( 2.55183673582591&gt;0,0.0535683073352875 +(0.0535683073352875*64.3646668942481),0)</f>
+        <v>3.5014745650597749</v>
+      </c>
+      <c r="M26" s="19">
         <f t="shared" si="2"/>
-        <v>96862.004613313416</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="21.75" customHeight="1">
+        <v>-11416.760734845768</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" s="34"/>
       <c r="C27" s="35"/>
       <c r="D27" s="10">
-        <v>9395</v>
+        <v>9142</v>
       </c>
       <c r="E27" s="10">
-        <v>2597</v>
+        <v>1140</v>
       </c>
       <c r="F27" s="10">
-        <v>8547</v>
+        <v>9220</v>
       </c>
       <c r="G27" s="10">
-        <v>7443</v>
-      </c>
-      <c r="H27" s="11">
+        <v>937</v>
+      </c>
+      <c r="H27" s="10">
+        <v>6079</v>
+      </c>
+      <c r="I27" s="11">
         <f t="shared" si="0"/>
-        <v>27982</v>
-      </c>
-      <c r="I27" s="12">
+        <v>26518</v>
+      </c>
+      <c r="J27" s="12">
         <f t="shared" si="1"/>
-        <v>0.1913233735598783</v>
-      </c>
-      <c r="J27" s="13">
-        <v>4.7296447934255204</v>
+        <v>0.12007570955063303</v>
       </c>
       <c r="K27" s="13">
-        <f>IF( 91.7931827212652&gt;0,4.72964479342552 + (4.72964479342552 * 91.7931827212652),0)</f>
-        <v>438.87879352301491</v>
-      </c>
-      <c r="L27" s="14">
+        <v>6.2650933564943703</v>
+      </c>
+      <c r="L27" s="13">
+        <f>IF( 54.87202212907&gt;0,6.26509335649437 + (6.26509335649437 * 54.87202212907),0)</f>
+        <v>350.0434346547429</v>
+      </c>
+      <c r="M27" s="14">
         <f t="shared" si="2"/>
-        <v>663752.19926244952</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A28" s="47" t="s">
-        <v>59</v>
-      </c>
+        <v>1357090.2772216427</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="47"/>
       <c r="B28" s="48"/>
       <c r="C28" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D28" s="16">
-        <v>5694</v>
+        <v>7141</v>
       </c>
       <c r="E28" s="16">
-        <v>2473</v>
+        <v>5081</v>
       </c>
       <c r="F28" s="16">
-        <v>6773</v>
+        <v>1584</v>
       </c>
       <c r="G28" s="16">
-        <v>7092</v>
+        <v>8590</v>
       </c>
       <c r="H28" s="16">
+        <v>9188</v>
+      </c>
+      <c r="I28" s="16">
         <f t="shared" si="0"/>
-        <v>22032</v>
-      </c>
-      <c r="I28" s="17">
+        <v>31584</v>
+      </c>
+      <c r="J28" s="17">
         <f t="shared" si="1"/>
-        <v>0.15064100372636832</v>
-      </c>
-      <c r="J28" s="18">
-        <v>0.477089787124232</v>
+        <v>0.14301497889913242</v>
       </c>
       <c r="K28" s="18">
-        <f>IF( 9.63866664079887&gt;0,0.477089787124232 +(0.477089787124232*54.0486428207013),0)</f>
-        <v>26.263145284806267</v>
-      </c>
-      <c r="L28" s="19">
+        <v>0.73206940839629098</v>
+      </c>
+      <c r="L28" s="18">
+        <f>IF( 2.83765808811302&gt;0,0.732069408396291 +(0.732069408396291*96.3874749822484),0)</f>
+        <v>71.294391195463177</v>
+      </c>
+      <c r="M28" s="19">
         <f t="shared" si="2"/>
-        <v>47744.766815854557</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="22.5" customHeight="1">
+        <v>130089.13642787049</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="47"/>
       <c r="B29" s="48"/>
       <c r="C29" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D29" s="16">
-        <v>1879</v>
+        <v>4257</v>
       </c>
       <c r="E29" s="16">
-        <v>3077</v>
+        <v>5184</v>
       </c>
       <c r="F29" s="16">
-        <v>7709</v>
+        <v>2130</v>
       </c>
       <c r="G29" s="16">
-        <v>4683</v>
+        <v>9012</v>
       </c>
       <c r="H29" s="16">
+        <v>470</v>
+      </c>
+      <c r="I29" s="16">
         <f t="shared" si="0"/>
-        <v>17348</v>
-      </c>
-      <c r="I29" s="17">
+        <v>21053</v>
+      </c>
+      <c r="J29" s="17">
         <f t="shared" si="1"/>
-        <v>0.11861474821373628</v>
-      </c>
-      <c r="J29" s="18">
-        <v>0.793268829953516</v>
+        <v>9.5329735016572784E-2</v>
       </c>
       <c r="K29" s="18">
-        <f>IF( 1.8228822256545&gt;0,0.793268829953516 +(0.793268829953516*72.130600536303),0)</f>
-        <v>58.012225921231057</v>
-      </c>
-      <c r="L29" s="19">
+        <v>0.90953230387975104</v>
+      </c>
+      <c r="L29" s="18">
+        <f>IF( 1.73138571052411&gt;0,0.909532303879751 +(0.909532303879751*38.0670504821777),0)</f>
+        <v>35.532744430841618</v>
+      </c>
+      <c r="M29" s="19">
         <f t="shared" si="2"/>
-        <v>98671.53272485148</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="22.5" customHeight="1">
+        <v>179811.75211801974</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="47"/>
       <c r="B30" s="48"/>
       <c r="C30" s="15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D30" s="16">
-        <v>2947</v>
+        <v>7169</v>
       </c>
       <c r="E30" s="16">
-        <v>783</v>
+        <v>7308</v>
       </c>
       <c r="F30" s="16">
-        <v>1206</v>
+        <v>3058</v>
       </c>
       <c r="G30" s="16">
-        <v>2011</v>
+        <v>7593</v>
       </c>
       <c r="H30" s="16">
+        <v>2217</v>
+      </c>
+      <c r="I30" s="16">
         <f t="shared" si="0"/>
-        <v>6947</v>
-      </c>
-      <c r="I30" s="17">
+        <v>27345</v>
+      </c>
+      <c r="J30" s="17">
         <f t="shared" si="1"/>
-        <v>4.7499230795528355E-2</v>
-      </c>
-      <c r="J30" s="18">
-        <v>0.31123508201503902</v>
+        <v>0.12382043433373784</v>
       </c>
       <c r="K30" s="18">
-        <f>IF( 4.40160419531241&gt;0,0.311235082015039 +(0.311235082015039*6.84288847578824),0)</f>
-        <v>2.4409820379967573</v>
-      </c>
-      <c r="L30" s="19">
+        <v>0.67315036462300903</v>
+      </c>
+      <c r="L30" s="18">
+        <f>IF( 2.88334918808348&gt;0,0.673150364623009 +(0.673150364623009*78.8661931542988),0)</f>
+        <v>53.761957042867905</v>
+      </c>
+      <c r="M30" s="19">
         <f t="shared" si="2"/>
-        <v>38572.686920109532</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="22.5" customHeight="1">
+        <v>121316.21912480381</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="47"/>
       <c r="B31" s="48"/>
       <c r="C31" s="15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D31" s="16">
-        <v>2852</v>
+        <v>266</v>
       </c>
       <c r="E31" s="16">
-        <v>7296</v>
+        <v>56</v>
       </c>
       <c r="F31" s="16">
-        <v>1685</v>
+        <v>52</v>
       </c>
       <c r="G31" s="16">
-        <v>3973</v>
+        <v>6115</v>
       </c>
       <c r="H31" s="16">
+        <v>1337</v>
+      </c>
+      <c r="I31" s="16">
         <f t="shared" si="0"/>
-        <v>15806</v>
-      </c>
-      <c r="I31" s="17">
+        <v>7826</v>
+      </c>
+      <c r="J31" s="17">
         <f t="shared" si="1"/>
-        <v>0.10807151892243</v>
-      </c>
-      <c r="J31" s="18">
-        <v>0.37231465073875802</v>
+        <v>3.5436778902754887E-2</v>
       </c>
       <c r="K31" s="18">
-        <f>IF( 6.88544718403623&gt;0,0.372314650738758 +(0.372314650738758*32.1336605735746),0)</f>
-        <v>12.336147264146986</v>
-      </c>
-      <c r="L31" s="19">
+        <v>0.40406567435900898</v>
+      </c>
+      <c r="L31" s="18">
+        <f>IF( 0.474665183794994&gt;0,0.404065674359009 +(0.404065674359009*25.4517585157658),0)</f>
+        <v>10.688247642654567</v>
+      </c>
+      <c r="M31" s="19">
         <f t="shared" si="2"/>
-        <v>38646.879243797055</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="21.75" customHeight="1">
+        <v>81409.479788140976</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="33" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B32" s="34"/>
       <c r="C32" s="35"/>
       <c r="D32" s="10">
-        <v>1417</v>
+        <v>1448</v>
       </c>
       <c r="E32" s="10">
-        <v>5769</v>
+        <v>883</v>
       </c>
       <c r="F32" s="10">
-        <v>8358</v>
+        <v>7975</v>
       </c>
       <c r="G32" s="10">
-        <v>3078</v>
-      </c>
-      <c r="H32" s="11">
+        <v>6267</v>
+      </c>
+      <c r="H32" s="10">
+        <v>9655</v>
+      </c>
+      <c r="I32" s="11">
         <f t="shared" si="0"/>
-        <v>18622</v>
-      </c>
-      <c r="I32" s="12">
+        <v>26228</v>
+      </c>
+      <c r="J32" s="12">
         <f t="shared" si="1"/>
-        <v>0.1273255615192643</v>
-      </c>
-      <c r="J32" s="13">
-        <v>7.8793639307279904</v>
+        <v>0.11876256543080184</v>
       </c>
       <c r="K32" s="13">
-        <f>IF( 45.2876914969122&gt;0,7.87936393072799 + (7.87936393072799 * 45.2876914969122),0)</f>
-        <v>364.71756681743472</v>
-      </c>
-      <c r="L32" s="14">
+        <v>1.0642305673399199</v>
+      </c>
+      <c r="L32" s="13">
+        <f>IF( 33.5717697318512&gt;0,1.06423056733992 + (1.06423056733992 * 33.5717697318512),0)</f>
+        <v>36.792334115673071</v>
+      </c>
+      <c r="M32" s="14">
         <f t="shared" si="2"/>
-        <v>1133774.3716886223</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A33" s="47" t="s">
-        <v>65</v>
-      </c>
+        <v>208800.93541361729</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="47"/>
       <c r="B33" s="48"/>
       <c r="C33" s="15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D33" s="16">
-        <v>3449</v>
+        <v>1368</v>
       </c>
       <c r="E33" s="16">
-        <v>4534</v>
+        <v>6760</v>
       </c>
       <c r="F33" s="16">
-        <v>3255</v>
+        <v>5360</v>
       </c>
       <c r="G33" s="16">
-        <v>6362</v>
+        <v>438</v>
       </c>
       <c r="H33" s="16">
+        <v>7427</v>
+      </c>
+      <c r="I33" s="16">
         <f t="shared" si="0"/>
-        <v>17600</v>
-      </c>
-      <c r="I33" s="17">
+        <v>21353</v>
+      </c>
+      <c r="J33" s="17">
         <f t="shared" si="1"/>
-        <v>0.12033776623021435</v>
-      </c>
-      <c r="J33" s="18">
-        <v>0.37020873481883099</v>
+        <v>9.66881599681223E-2</v>
       </c>
       <c r="K33" s="18">
-        <f>IF( 1.04677111890482&gt;0,0.370208734818831 +(0.370208734818831*19.0733177210546),0)</f>
-        <v>7.4313175571280432</v>
-      </c>
-      <c r="L33" s="19">
+        <v>0.58039011321048695</v>
+      </c>
+      <c r="L33" s="18">
+        <f>IF( 6.39187917410949&gt;0,0.580390113210487 +(0.580390113210487*59.0762932594289),0)</f>
+        <v>34.86768664610635</v>
+      </c>
+      <c r="M33" s="19">
         <f t="shared" si="2"/>
-        <v>36544.878510928123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="22.5" customHeight="1">
+        <v>106822.67416185678</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="47"/>
       <c r="B34" s="48"/>
       <c r="C34" s="15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D34" s="16">
-        <v>5334</v>
+        <v>5331</v>
       </c>
       <c r="E34" s="16">
-        <v>3322</v>
+        <v>3890</v>
       </c>
       <c r="F34" s="16">
-        <v>9560</v>
+        <v>1915</v>
       </c>
       <c r="G34" s="16">
-        <v>2039</v>
+        <v>7796</v>
       </c>
       <c r="H34" s="16">
+        <v>8450</v>
+      </c>
+      <c r="I34" s="16">
         <f t="shared" si="0"/>
-        <v>20255</v>
-      </c>
-      <c r="I34" s="17">
+        <v>27382</v>
+      </c>
+      <c r="J34" s="17">
         <f t="shared" si="1"/>
-        <v>0.13849099176096544</v>
-      </c>
-      <c r="J34" s="18">
-        <v>0.75165847397952301</v>
+        <v>0.12398797341109562</v>
       </c>
       <c r="K34" s="18">
-        <f>IF( 6.23928787942943&gt;0,0.751658473979523 +(0.751658473979523*77.4870735488306),0)</f>
-        <v>58.995473930832588</v>
-      </c>
-      <c r="L34" s="19">
+        <v>0.70741505534733395</v>
+      </c>
+      <c r="L34" s="18">
+        <f>IF( 0.407251417826513&gt;0,0.707415055347334 +(0.707415055347334*21.9290482448084),0)</f>
+        <v>16.220353933162823</v>
+      </c>
+      <c r="M34" s="19">
         <f t="shared" si="2"/>
-        <v>89678.810111875136</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="22.5" customHeight="1">
+        <v>128846.37048312661</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="47"/>
       <c r="B35" s="48"/>
       <c r="C35" s="15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D35" s="16">
-        <v>8193</v>
+        <v>3695</v>
       </c>
       <c r="E35" s="16">
-        <v>529</v>
+        <v>8333</v>
       </c>
       <c r="F35" s="16">
-        <v>5424</v>
+        <v>9141</v>
       </c>
       <c r="G35" s="16">
-        <v>3023</v>
+        <v>7280</v>
       </c>
       <c r="H35" s="16">
+        <v>6729</v>
+      </c>
+      <c r="I35" s="16">
         <f t="shared" si="0"/>
-        <v>17169</v>
-      </c>
-      <c r="I35" s="17">
+        <v>35178</v>
+      </c>
+      <c r="J35" s="17">
         <f t="shared" si="1"/>
-        <v>0.11739085843219035</v>
-      </c>
-      <c r="J35" s="18">
-        <v>0.81070386842391595</v>
+        <v>0.15928890981869556</v>
       </c>
       <c r="K35" s="18">
-        <f>IF( 2.84448401203588&gt;0,0.810703868423916 +(0.810703868423916*51.7222690636861),0)</f>
-        <v>42.742147482016868</v>
-      </c>
-      <c r="L35" s="19">
+        <v>0.83102355284198304</v>
+      </c>
+      <c r="L35" s="18">
+        <f>IF( 0.21129327836041&gt;0,0.831023552841983 +(0.831023552841983*47.0535293440584),0)</f>
+        <v>39.933614682095893</v>
+      </c>
+      <c r="M35" s="19">
         <f t="shared" si="2"/>
-        <v>101400.49427633983</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A36" s="47"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="16">
-        <v>5097</v>
-      </c>
-      <c r="E36" s="16">
-        <v>3129</v>
-      </c>
-      <c r="F36" s="16">
-        <v>1056</v>
-      </c>
-      <c r="G36" s="16">
-        <v>2760</v>
-      </c>
-      <c r="H36" s="16">
+        <v>148348.56550383489</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="34"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="10">
+        <v>5544</v>
+      </c>
+      <c r="E36" s="10">
+        <v>465</v>
+      </c>
+      <c r="F36" s="10">
+        <v>3085</v>
+      </c>
+      <c r="G36" s="10">
+        <v>9220</v>
+      </c>
+      <c r="H36" s="10">
+        <v>1165</v>
+      </c>
+      <c r="I36" s="11">
         <f t="shared" si="0"/>
-        <v>12042</v>
-      </c>
-      <c r="I36" s="17">
+        <v>19479</v>
+      </c>
+      <c r="J36" s="12">
         <f t="shared" si="1"/>
-        <v>8.2335646644559154E-2</v>
-      </c>
-      <c r="J36" s="18">
-        <v>0.21914982247126699</v>
-      </c>
-      <c r="K36" s="18">
-        <f>IF( 3.99208995233853&gt;0,0.219149822471267 +(0.219149822471267*85.4214908021602),0)</f>
-        <v>18.939254366995641</v>
-      </c>
-      <c r="L36" s="19">
+        <v>8.8202532104109693E-2</v>
+      </c>
+      <c r="K36" s="13">
+        <v>9.5777742609278196</v>
+      </c>
+      <c r="L36" s="13">
+        <f>IF( 79.473589863383&gt;0,9.57777426092782 + (9.57777426092782 * 79.473589863383),0)</f>
+        <v>770.75787767797158</v>
+      </c>
+      <c r="M36" s="14">
         <f t="shared" si="2"/>
-        <v>20009.757285535154</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A37" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="10">
-        <v>3545</v>
-      </c>
-      <c r="E37" s="10">
-        <v>4262</v>
-      </c>
-      <c r="F37" s="10">
-        <v>3097</v>
-      </c>
-      <c r="G37" s="10">
-        <v>7357</v>
-      </c>
-      <c r="H37" s="11">
+        <v>2095714.9788803435</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="47"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="16">
+        <v>1611</v>
+      </c>
+      <c r="E37" s="16">
+        <v>859</v>
+      </c>
+      <c r="F37" s="16">
+        <v>9974</v>
+      </c>
+      <c r="G37" s="16">
+        <v>7530</v>
+      </c>
+      <c r="H37" s="16">
+        <v>7460</v>
+      </c>
+      <c r="I37" s="16">
         <f t="shared" si="0"/>
-        <v>18261</v>
-      </c>
-      <c r="I37" s="12">
+        <v>27434</v>
+      </c>
+      <c r="J37" s="17">
         <f t="shared" si="1"/>
-        <v>0.12485726983692866</v>
-      </c>
-      <c r="J37" s="13">
-        <v>1.8684562583772699</v>
-      </c>
-      <c r="K37" s="13">
-        <f>IF( 33.4784743066311&gt;0,1.86845625837727 + (1.86845625837727 * 33.4784743066311),0)</f>
-        <v>64.421521097524774</v>
-      </c>
-      <c r="L37" s="14">
+        <v>0.12422343373603087</v>
+      </c>
+      <c r="K37" s="18">
+        <v>0.28319258535429498</v>
+      </c>
+      <c r="L37" s="18">
+        <f>IF( 4.24309876479353&gt;0,0.283192585354295 +(0.283192585354295*36.5078307392578),0)</f>
+        <v>10.621939558081712</v>
+      </c>
+      <c r="M37" s="19">
         <f t="shared" si="2"/>
-        <v>255010.07006896759</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A38" s="47" t="s">
-        <v>71</v>
-      </c>
+        <v>35107.383319983921</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="47"/>
       <c r="B38" s="48"/>
       <c r="C38" s="15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D38" s="16">
-        <v>8755</v>
+        <v>213</v>
       </c>
       <c r="E38" s="16">
-        <v>6756</v>
+        <v>6005</v>
       </c>
       <c r="F38" s="16">
-        <v>708</v>
+        <v>166</v>
       </c>
       <c r="G38" s="16">
-        <v>9637</v>
+        <v>8569</v>
       </c>
       <c r="H38" s="16">
+        <v>4755</v>
+      </c>
+      <c r="I38" s="16">
         <f t="shared" si="0"/>
-        <v>25856</v>
-      </c>
-      <c r="I38" s="17">
+        <v>19708</v>
+      </c>
+      <c r="J38" s="17">
         <f t="shared" si="1"/>
-        <v>0.1767871183891149</v>
-      </c>
-      <c r="J38" s="18">
-        <v>9.3837170439696499E-2</v>
+        <v>8.923946315045915E-2</v>
       </c>
       <c r="K38" s="18">
-        <f>IF( 1.96449013518379&gt;0,0.0938371704396965 +(0.0938371704396965*83.6123108787519),0)</f>
-        <v>7.9397798372260286</v>
-      </c>
-      <c r="L38" s="19">
+        <v>0.261532220179929</v>
+      </c>
+      <c r="L38" s="18">
+        <f>IF( 6.28302641971178&gt;0,0.261532220179929 +(0.261532220179929*31.8838966227527),0)</f>
+        <v>8.6001984919157817</v>
+      </c>
+      <c r="M38" s="19">
         <f t="shared" si="2"/>
-        <v>-12131.844637342188</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A39" s="47"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="16">
-        <v>4413</v>
-      </c>
-      <c r="E39" s="16">
-        <v>1699</v>
-      </c>
-      <c r="F39" s="16">
-        <v>9369</v>
-      </c>
-      <c r="G39" s="16">
-        <v>6977</v>
-      </c>
-      <c r="H39" s="16">
+        <v>38049.821633416243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="34"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="10">
+        <v>7118</v>
+      </c>
+      <c r="E39" s="10">
+        <v>2449</v>
+      </c>
+      <c r="F39" s="10">
+        <v>9269</v>
+      </c>
+      <c r="G39" s="10">
+        <v>3118</v>
+      </c>
+      <c r="H39" s="10">
+        <v>6580</v>
+      </c>
+      <c r="I39" s="11">
         <f t="shared" si="0"/>
-        <v>22458</v>
-      </c>
-      <c r="I39" s="17">
+        <v>28534</v>
+      </c>
+      <c r="J39" s="12">
         <f t="shared" si="1"/>
-        <v>0.15355372465898601</v>
-      </c>
-      <c r="J39" s="18">
-        <v>1.30656575844929E-2</v>
-      </c>
-      <c r="K39" s="18">
-        <f>IF( 6.33667507038297&gt;0,0.0130656575844929 +(0.0130656575844929*53.1924676863442),0)</f>
-        <v>0.70806022644846944</v>
-      </c>
-      <c r="L39" s="19">
+        <v>0.12920432522504574</v>
+      </c>
+      <c r="K39" s="13">
+        <v>9.1690152739961697</v>
+      </c>
+      <c r="L39" s="13">
+        <f>IF( 71.018837099438&gt;0,9.16901527399617 + (9.16901527399617 * 71.018837099438),0)</f>
+        <v>660.34181738018901</v>
+      </c>
+      <c r="M39" s="14">
         <f t="shared" si="2"/>
-        <v>-20547.082249979991</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="22.5" customHeight="1">
+        <v>1996388.00917041</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="47"/>
       <c r="B40" s="48"/>
       <c r="C40" s="15" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D40" s="16">
-        <v>5914</v>
+        <v>860</v>
       </c>
       <c r="E40" s="16">
-        <v>2717</v>
+        <v>9478</v>
       </c>
       <c r="F40" s="16">
-        <v>244</v>
+        <v>8701</v>
       </c>
       <c r="G40" s="16">
-        <v>174</v>
+        <v>901</v>
       </c>
       <c r="H40" s="16">
+        <v>5542</v>
+      </c>
+      <c r="I40" s="16">
         <f t="shared" si="0"/>
-        <v>9049</v>
-      </c>
-      <c r="I40" s="17">
+        <v>25482</v>
+      </c>
+      <c r="J40" s="17">
         <f t="shared" si="1"/>
-        <v>6.187138901234146E-2</v>
-      </c>
-      <c r="J40" s="18">
-        <v>0.47396216470467001</v>
+        <v>0.11538461538461539</v>
       </c>
       <c r="K40" s="18">
-        <f>IF( 8.35002756600735&gt;0,0.47396216470467 +(0.47396216470467*14.0688081803121),0)</f>
-        <v>7.1420449446601619</v>
-      </c>
-      <c r="L40" s="19">
+        <v>0.23119695867933199</v>
+      </c>
+      <c r="L40" s="18">
+        <f>IF( 4.67208837376539&gt;0,0.231196958679332 +(0.231196958679332*8.31133118286325),0)</f>
+        <v>2.1527514507340104</v>
+      </c>
+      <c r="M40" s="19">
         <f t="shared" si="2"/>
-        <v>60270.336398881511</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
+        <v>25576.461142578395</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="33" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B41" s="34"/>
       <c r="C41" s="35"/>
       <c r="D41" s="10">
-        <v>14322</v>
+        <v>528</v>
       </c>
       <c r="E41" s="10">
-        <v>9995</v>
+        <v>4718</v>
       </c>
       <c r="F41" s="10">
-        <v>4667</v>
+        <v>6269</v>
       </c>
       <c r="G41" s="10">
-        <v>3442</v>
-      </c>
-      <c r="H41" s="11">
+        <v>5545</v>
+      </c>
+      <c r="H41" s="10">
+        <v>4948</v>
+      </c>
+      <c r="I41" s="11">
         <f t="shared" si="0"/>
-        <v>32426</v>
-      </c>
-      <c r="I41" s="12"/>
-      <c r="J41" s="13"/>
+        <v>22008</v>
+      </c>
+      <c r="J41" s="12">
+        <f t="shared" si="1"/>
+        <v>9.9654054445672061E-2</v>
+      </c>
       <c r="K41" s="13">
-        <f>IF( 36.055730998542&gt;0,2.20116829136441 + 2.20116829136441 * 15.1058912347564,0)</f>
-        <v>35.451777090109772</v>
-      </c>
-      <c r="L41" s="14"/>
-    </row>
-    <row r="42" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A42" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B42" s="34"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="10">
-        <v>5933</v>
-      </c>
-      <c r="E42" s="10">
-        <v>13050</v>
-      </c>
-      <c r="F42" s="10">
-        <v>17658</v>
-      </c>
-      <c r="G42" s="10">
-        <v>2872</v>
-      </c>
-      <c r="H42" s="11">
+        <v>4.3945138921935598</v>
+      </c>
+      <c r="L41" s="13">
+        <f>IF( 68.4604351261912&gt;0,4.39451389219356 + (4.39451389219356 * 68.4604351261912),0)</f>
+        <v>305.24484711985679</v>
+      </c>
+      <c r="M41" s="14">
+        <f t="shared" si="2"/>
+        <v>948494.02600759454</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="47"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="16">
+        <v>6525</v>
+      </c>
+      <c r="E42" s="16">
+        <v>2316</v>
+      </c>
+      <c r="F42" s="16">
+        <v>64</v>
+      </c>
+      <c r="G42" s="16">
+        <v>6141</v>
+      </c>
+      <c r="H42" s="16">
+        <v>4832</v>
+      </c>
+      <c r="I42" s="16">
         <f t="shared" si="0"/>
-        <v>39513</v>
-      </c>
-      <c r="I42" s="12"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13">
-        <f>IF( 33.6518269188943&gt;0,7.05468116656629 + 7.05468116656629 * 34.6111144566029,0)</f>
-        <v>251.22505847743301</v>
-      </c>
-      <c r="L42" s="14"/>
-    </row>
-    <row r="43" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A43" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43" s="34"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="10">
-        <v>14759</v>
-      </c>
-      <c r="E43" s="10">
-        <v>3674</v>
-      </c>
-      <c r="F43" s="10">
-        <v>11435</v>
-      </c>
-      <c r="G43" s="10">
-        <v>7565</v>
-      </c>
-      <c r="H43" s="11">
+        <v>19878</v>
+      </c>
+      <c r="J42" s="17">
+        <f t="shared" si="1"/>
+        <v>9.0009237289670543E-2</v>
+      </c>
+      <c r="K42" s="18">
+        <v>0.53320367845390204</v>
+      </c>
+      <c r="L42" s="18">
+        <f>IF( 0.820988831492601&gt;0,0.533203678453902 +(0.533203678453902*23.1129229642045),0)</f>
+        <v>12.857099222789406</v>
+      </c>
+      <c r="M42" s="19">
+        <f t="shared" si="2"/>
+        <v>97876.833164473544</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="47"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="16">
+        <v>1209</v>
+      </c>
+      <c r="E43" s="16">
+        <v>5917</v>
+      </c>
+      <c r="F43" s="16">
+        <v>9590</v>
+      </c>
+      <c r="G43" s="16">
+        <v>3992</v>
+      </c>
+      <c r="H43" s="16">
+        <v>1035</v>
+      </c>
+      <c r="I43" s="16">
         <f t="shared" si="0"/>
-        <v>37433</v>
-      </c>
-      <c r="I43" s="12"/>
-      <c r="J43" s="13"/>
-      <c r="K43" s="13">
-        <f>IF( 73.5425582032383&gt;0,9.96819677295545 + 9.96819677295545 * 85.5095433935102,0)</f>
-        <v>862.34415128503781</v>
-      </c>
-      <c r="L43" s="14"/>
-    </row>
-    <row r="44" spans="1:12" ht="22.5" customHeight="1">
+        <v>21743</v>
+      </c>
+      <c r="J43" s="17">
+        <f t="shared" si="1"/>
+        <v>9.8454112405136657E-2</v>
+      </c>
+      <c r="K43" s="18">
+        <v>0.234029956736616</v>
+      </c>
+      <c r="L43" s="18">
+        <f>IF( 7.80157579938023&gt;0,0.234029956736616 +(0.234029956736616*34.2916004985066),0)</f>
+        <v>8.2592917378314343</v>
+      </c>
+      <c r="M43" s="19">
+        <f t="shared" si="2"/>
+        <v>29941.111765541224</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="33" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B44" s="34"/>
       <c r="C44" s="35"/>
       <c r="D44" s="10">
-        <v>4962</v>
+        <v>9946</v>
       </c>
       <c r="E44" s="10">
-        <v>10031</v>
+        <v>12766</v>
       </c>
       <c r="F44" s="10">
-        <v>11455</v>
+        <v>12978</v>
       </c>
       <c r="G44" s="10">
-        <v>10435</v>
-      </c>
-      <c r="H44" s="11">
+        <v>5524</v>
+      </c>
+      <c r="H44" s="10">
+        <v>16454</v>
+      </c>
+      <c r="I44" s="11">
         <f t="shared" si="0"/>
-        <v>36883</v>
-      </c>
-      <c r="I44" s="12"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13">
-        <f>IF( 32.1110604014765&gt;0,3.31253189282144 + 3.31253189282144 * 4.17850953721372,0)</f>
-        <v>17.153977999300441</v>
-      </c>
-      <c r="L44" s="14"/>
-    </row>
-    <row r="45" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A45" s="36" t="s">
+        <v>57668</v>
+      </c>
+      <c r="J44" s="12"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13">
+        <f>IF( 66.0662032971467&gt;0,6.87737221218523 + 6.87737221218523 * 33.5440770413466,0)</f>
+        <v>237.57247553974287</v>
+      </c>
+      <c r="M44" s="14"/>
+    </row>
+    <row r="45" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="34"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="10">
+        <v>18183</v>
+      </c>
+      <c r="E45" s="10">
+        <v>13437</v>
+      </c>
+      <c r="F45" s="10">
+        <v>14812</v>
+      </c>
+      <c r="G45" s="10">
+        <v>11876</v>
+      </c>
+      <c r="H45" s="10">
+        <v>4109</v>
+      </c>
+      <c r="I45" s="11">
+        <f t="shared" si="0"/>
+        <v>62417</v>
+      </c>
+      <c r="J45" s="12"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13">
+        <f>IF( 27.5858585851201&gt;0,5.54321288389303 + 5.54321288389303 * 46.6602779676487,0)</f>
+        <v>264.19106688019343</v>
+      </c>
+      <c r="M45" s="14"/>
+    </row>
+    <row r="46" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="34"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="10">
+        <v>10590</v>
+      </c>
+      <c r="E46" s="10">
+        <v>2023</v>
+      </c>
+      <c r="F46" s="10">
+        <v>17195</v>
+      </c>
+      <c r="G46" s="10">
+        <v>7204</v>
+      </c>
+      <c r="H46" s="10">
+        <v>15734</v>
+      </c>
+      <c r="I46" s="11">
+        <f t="shared" si="0"/>
+        <v>52746</v>
+      </c>
+      <c r="J46" s="12"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13">
+        <f>IF( 54.8418879298688&gt;0,3.68940522134742 + 3.68940522134742 * 77.3651561594406,0)</f>
+        <v>289.12081630634611</v>
+      </c>
+      <c r="M46" s="14"/>
+    </row>
+    <row r="47" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="34"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="10">
+        <v>12662</v>
+      </c>
+      <c r="E47" s="10">
+        <v>2914</v>
+      </c>
+      <c r="F47" s="10">
+        <v>12354</v>
+      </c>
+      <c r="G47" s="10">
+        <v>12338</v>
+      </c>
+      <c r="H47" s="10">
+        <v>7745</v>
+      </c>
+      <c r="I47" s="11">
+        <f t="shared" si="0"/>
+        <v>48013</v>
+      </c>
+      <c r="J47" s="12"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13">
+        <f>IF( 57.6927868918017&gt;0,0.356100779192569 + 0.356100779192569 * 0.595758576223514,0)</f>
+        <v>0.56825087239641792</v>
+      </c>
+      <c r="M47" s="14"/>
+    </row>
+    <row r="48" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="37"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="20">
-        <f>SUM(D41:D44)</f>
-        <v>39976</v>
-      </c>
-      <c r="E45" s="20">
-        <f>SUM(E41:E44)</f>
-        <v>36750</v>
-      </c>
-      <c r="F45" s="20">
-        <f>SUM(F41:F44)</f>
-        <v>45215</v>
-      </c>
-      <c r="G45" s="20">
-        <f>SUM(G41:G44)</f>
-        <v>24314</v>
-      </c>
-      <c r="H45" s="21">
+      <c r="B48" s="37"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="20">
+        <f>SUM(D44:D47)</f>
+        <v>51381</v>
+      </c>
+      <c r="E48" s="20">
+        <f>SUM(E44:E47)</f>
+        <v>31140</v>
+      </c>
+      <c r="F48" s="20">
+        <f>SUM(F44:F47)</f>
+        <v>57339</v>
+      </c>
+      <c r="G48" s="20">
+        <f>SUM(G44:G47)</f>
+        <v>36942</v>
+      </c>
+      <c r="H48" s="20">
+        <f>SUM(H44:H47)</f>
+        <v>44042</v>
+      </c>
+      <c r="I48" s="21">
         <f t="shared" si="0"/>
-        <v>146255</v>
-      </c>
-      <c r="I45" s="22">
-        <f>SUM(I8:I40)</f>
-        <v>3.8161020136063732</v>
-      </c>
-      <c r="J45" s="23"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="24"/>
-    </row>
-    <row r="46" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A46" s="42" t="s">
+        <v>220844</v>
+      </c>
+      <c r="J48" s="22">
+        <f>SUM(J8:J43)</f>
+        <v>3.9293845429352841</v>
+      </c>
+      <c r="K48" s="23"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="24"/>
+    </row>
+    <row r="49" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="43"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="25">
-        <f>D45/H45</f>
-        <v>0.27333082629653688</v>
-      </c>
-      <c r="E46" s="25">
-        <f>E45/H45</f>
-        <v>0.25127346073638507</v>
-      </c>
-      <c r="F46" s="25">
-        <f>F45/H45</f>
-        <v>0.30915182386926943</v>
-      </c>
-      <c r="G46" s="25">
-        <f>G45/H45</f>
-        <v>0.16624388909780863</v>
-      </c>
-      <c r="H46" s="26"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
-      <c r="L46" s="25"/>
-    </row>
-    <row r="47" spans="1:12" s="3" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A47" s="45"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-    </row>
-    <row r="48" spans="1:12" s="3" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A48" s="46"/>
-      <c r="B48" s="46"/>
-      <c r="C48" s="46"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-    </row>
-    <row r="49" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A49" s="39" t="s">
+      <c r="B49" s="43"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="25">
+        <f>D48/I48</f>
+        <v>0.23265744145188458</v>
+      </c>
+      <c r="E49" s="25">
+        <f>E48/I48</f>
+        <v>0.14100450997083913</v>
+      </c>
+      <c r="F49" s="25">
+        <f>F48/I48</f>
+        <v>0.25963576098965785</v>
+      </c>
+      <c r="G49" s="25">
+        <f>G48/I48</f>
+        <v>0.16727644853380666</v>
+      </c>
+      <c r="H49" s="25">
+        <f>H48/I48</f>
+        <v>0.19942583905381175</v>
+      </c>
+      <c r="I49" s="26"/>
+      <c r="J49" s="25"/>
+      <c r="K49" s="25"/>
+      <c r="L49" s="25"/>
+      <c r="M49" s="25"/>
+    </row>
+    <row r="50" spans="1:13" s="3" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="45"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="31"/>
+    </row>
+    <row r="51" spans="1:13" s="3" customFormat="1" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="46"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+    </row>
+    <row r="52" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="40"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="27">
-        <v>6733</v>
-      </c>
-      <c r="E49" s="27">
-        <v>8616</v>
-      </c>
-      <c r="F49" s="27">
-        <v>8741</v>
-      </c>
-      <c r="G49" s="27">
-        <v>1484</v>
-      </c>
-      <c r="H49" s="28">
-        <f>SUM(D49:G49)</f>
-        <v>25574</v>
-      </c>
-      <c r="I49" s="29"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="30"/>
-      <c r="L49" s="30"/>
-    </row>
-    <row r="50" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A50" s="39" t="s">
+      <c r="B52" s="40"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="27">
+        <v>9341</v>
+      </c>
+      <c r="E52" s="27">
+        <v>8982</v>
+      </c>
+      <c r="F52" s="27">
+        <v>7802</v>
+      </c>
+      <c r="G52" s="27">
+        <v>2634</v>
+      </c>
+      <c r="H52" s="27">
+        <v>7954</v>
+      </c>
+      <c r="I52" s="28">
+        <f>SUM(D52:H52)</f>
+        <v>36713</v>
+      </c>
+      <c r="J52" s="29"/>
+      <c r="K52" s="30"/>
+      <c r="L52" s="30"/>
+      <c r="M52" s="30"/>
+    </row>
+    <row r="53" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="40"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="27">
-        <v>5963</v>
-      </c>
-      <c r="E50" s="27">
-        <v>3387</v>
-      </c>
-      <c r="F50" s="27">
-        <v>7211</v>
-      </c>
-      <c r="G50" s="27">
-        <v>8663</v>
-      </c>
-      <c r="H50" s="28">
-        <f>SUM(D50:G50)</f>
-        <v>25224</v>
-      </c>
-      <c r="I50" s="29"/>
-      <c r="J50" s="30"/>
-      <c r="K50" s="30"/>
-      <c r="L50" s="30"/>
-    </row>
-    <row r="51" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A51" s="39" t="s">
+      <c r="B53" s="40"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="27">
+        <v>239</v>
+      </c>
+      <c r="E53" s="27">
+        <v>6473</v>
+      </c>
+      <c r="F53" s="27">
+        <v>5265</v>
+      </c>
+      <c r="G53" s="27">
+        <v>5102</v>
+      </c>
+      <c r="H53" s="27">
+        <v>2221</v>
+      </c>
+      <c r="I53" s="28">
+        <f>SUM(D53:H53)</f>
+        <v>19300</v>
+      </c>
+      <c r="J53" s="29"/>
+      <c r="K53" s="30"/>
+      <c r="L53" s="30"/>
+      <c r="M53" s="30"/>
+    </row>
+    <row r="54" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="40"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="27">
-        <v>4039</v>
-      </c>
-      <c r="E51" s="27">
-        <v>9928</v>
-      </c>
-      <c r="F51" s="27">
-        <v>2678</v>
-      </c>
-      <c r="G51" s="27">
-        <v>7826</v>
-      </c>
-      <c r="H51" s="28">
-        <f>SUM(D51:G51)</f>
-        <v>24471</v>
-      </c>
-      <c r="I51" s="29"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="30"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="27">
+        <v>384</v>
+      </c>
+      <c r="E54" s="27">
+        <v>6232</v>
+      </c>
+      <c r="F54" s="27">
+        <v>2296</v>
+      </c>
+      <c r="G54" s="27">
+        <v>8493</v>
+      </c>
+      <c r="H54" s="27">
+        <v>9800</v>
+      </c>
+      <c r="I54" s="28">
+        <f>SUM(D54:H54)</f>
+        <v>27205</v>
+      </c>
+      <c r="J54" s="29"/>
+      <c r="K54" s="30"/>
+      <c r="L54" s="30"/>
+      <c r="M54" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="A38:B40"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:B31"/>
+  <mergeCells count="37">
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:B43"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A46:C46"/>
     <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:B36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="A33:B35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="A39:C39"/>
     <mergeCell ref="K5:K7"/>
     <mergeCell ref="L5:L7"/>
+    <mergeCell ref="M5:M7"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="A5:C7"/>
-    <mergeCell ref="H5:H7"/>
     <mergeCell ref="I5:I7"/>
+    <mergeCell ref="J5:J7"/>
     <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A54:C54"/>
     <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A47:D48"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A11:B13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:B18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A50:D51"/>
+    <mergeCell ref="A9:B12"/>
+    <mergeCell ref="A14:B16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:B21"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A23:B26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:B31"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.5" header="0.5" footer="0.25"/>
@@ -3250,19 +4108,20 @@
   <headerFooter>
     <oddFooter>&amp;R&amp;G</oddFooter>
   </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawingHF r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A288C8-8FE1-44E0-ACFA-D6DB1FEB56F3}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
@@ -3275,7 +4134,7 @@
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -3304,12 +4163,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2">
@@ -3329,12 +4188,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2">
@@ -3354,12 +4213,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2">
@@ -3379,12 +4238,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2">
@@ -3404,12 +4263,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
@@ -3429,12 +4288,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2">

</xml_diff>